<commit_message>
cambio en orden felpa
</commit_message>
<xml_diff>
--- a/app/Http/Controllers/OrdenDeCambio/Felpa/ordfelpa.xlsx
+++ b/app/Http/Controllers/OrdenDeCambio/Felpa/ordfelpa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsanchez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB25D4B2-73B3-42A5-A527-23EF47FF097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD6E88-C980-4348-94B1-37D8464E1B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5AD2B563-86DE-4E16-A95C-13676F9A1017}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5AD2B563-86DE-4E16-A95C-13676F9A1017}"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRO" sheetId="2" r:id="rId1"/>
@@ -1450,7 +1450,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="320">
+  <cellXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1835,9 +1835,8 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -2208,6 +2207,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2220,15 +2228,6 @@
     <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2283,15 +2282,15 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2316,7 +2315,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Millares 14" xfId="3" xr:uid="{FF4AF82A-FE93-4F17-B802-426D6F9A766B}"/>
@@ -4468,14 +4466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9094078E-86F1-4EC4-8CB6-4E162C7CAFAB}">
   <dimension ref="M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="4" spans="13:13">
-      <c r="M4" s="319"/>
+      <c r="M4" s="157"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4486,12 +4484,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AA01A9-D004-43E2-A15D-563D681279D3}">
   <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
     <col min="16" max="16" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4530,9 +4530,9 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="189"/>
-      <c r="O2" s="189"/>
-      <c r="P2" s="189"/>
+      <c r="N2" s="188"/>
+      <c r="O2" s="188"/>
+      <c r="P2" s="188"/>
     </row>
     <row r="3" spans="1:16" ht="14.4" customHeight="1">
       <c r="A3" s="1"/>
@@ -4540,13 +4540,13 @@
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="190" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="190"/>
-      <c r="H3" s="190"/>
-      <c r="I3" s="190"/>
-      <c r="J3" s="190"/>
+      <c r="F3" s="189" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="189"/>
+      <c r="H3" s="189"/>
+      <c r="I3" s="189"/>
+      <c r="J3" s="189"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -4560,11 +4560,11 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="190"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="190"/>
+      <c r="F4" s="189"/>
+      <c r="G4" s="189"/>
+      <c r="H4" s="189"/>
+      <c r="I4" s="189"/>
+      <c r="J4" s="189"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -4572,22 +4572,22 @@
       <c r="O4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="191">
+      <c r="P4" s="190">
         <f>[1]REGISTRO!A14</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.6" customHeight="1">
-      <c r="A5" s="192" t="s">
+      <c r="A5" s="191" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="192"/>
-      <c r="C5" s="192"/>
-      <c r="D5" s="193">
+      <c r="B5" s="191"/>
+      <c r="C5" s="191"/>
+      <c r="D5" s="192">
         <f ca="1">NOW()</f>
-        <v>45994.663394907409</v>
-      </c>
-      <c r="E5" s="193"/>
+        <v>46020.878260300924</v>
+      </c>
+      <c r="E5" s="192"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -4598,47 +4598,47 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="191"/>
+      <c r="P5" s="190"/>
     </row>
     <row r="6" spans="1:16" ht="15.6">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="162"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="167">
+      <c r="B6" s="161"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="166">
         <f>[1]REGISTRO!B14</f>
         <v>0</v>
       </c>
-      <c r="E6" s="167"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="166"/>
+      <c r="F6" s="163" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="164"/>
-      <c r="H6" s="164"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="194">
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="193">
         <f>[1]REGISTRO!F14</f>
         <v>0</v>
       </c>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
-      <c r="N6" s="194"/>
-      <c r="O6" s="194"/>
-      <c r="P6" s="194"/>
+      <c r="K6" s="193"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
+      <c r="P6" s="193"/>
     </row>
     <row r="7" spans="1:16" ht="15.6">
-      <c r="A7" s="162" t="s">
+      <c r="A7" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="163" t="e">
+      <c r="B7" s="161"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="162" t="e">
         <f>REGISTRO!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="E7" s="163"/>
+      <c r="E7" s="162"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
@@ -4648,18 +4648,18 @@
         <f>[1]REGISTRO!E14</f>
         <v>0</v>
       </c>
-      <c r="J7" s="164" t="s">
+      <c r="J7" s="163" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="164"/>
-      <c r="L7" s="165">
+      <c r="K7" s="163"/>
+      <c r="L7" s="164">
         <f>[1]REGISTRO!G14</f>
         <v>0</v>
       </c>
-      <c r="M7" s="165"/>
-      <c r="N7" s="165"/>
-      <c r="O7" s="165"/>
-      <c r="P7" s="165"/>
+      <c r="M7" s="164"/>
+      <c r="N7" s="164"/>
+      <c r="O7" s="164"/>
+      <c r="P7" s="164"/>
     </row>
     <row r="8" spans="1:16" ht="18">
       <c r="A8" s="10" t="s">
@@ -4667,30 +4667,30 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="166">
+      <c r="D8" s="165">
         <f>[1]REGISTRO!O14</f>
         <v>0</v>
       </c>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
       <c r="G8" s="11"/>
       <c r="H8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="167">
+      <c r="I8" s="166">
         <f>[1]REGISTRO!L14</f>
         <v>0</v>
       </c>
-      <c r="J8" s="167"/>
+      <c r="J8" s="166"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="168">
+      <c r="L8" s="167">
         <f>[1]REGISTRO!M14</f>
         <v>0</v>
       </c>
-      <c r="M8" s="168"/>
-      <c r="N8" s="168"/>
-      <c r="O8" s="168"/>
-      <c r="P8" s="168"/>
+      <c r="M8" s="167"/>
+      <c r="N8" s="167"/>
+      <c r="O8" s="167"/>
+      <c r="P8" s="167"/>
     </row>
     <row r="9" spans="1:16" ht="30">
       <c r="A9" s="10" t="s">
@@ -4701,27 +4701,27 @@
         <v>0</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="183" t="s">
+      <c r="D9" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="183"/>
+      <c r="E9" s="182"/>
       <c r="F9" s="13">
         <f>[1]REGISTRO!J14</f>
         <v>0</v>
       </c>
-      <c r="G9" s="184" t="s">
+      <c r="G9" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="184"/>
+      <c r="H9" s="183"/>
       <c r="I9" s="14">
         <f>[1]REGISTRO!AV14</f>
         <v>0</v>
       </c>
-      <c r="J9" s="185" t="s">
+      <c r="J9" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="185"/>
-      <c r="L9" s="185"/>
+      <c r="K9" s="184"/>
+      <c r="L9" s="184"/>
       <c r="M9" s="15">
         <f>[1]REGISTRO!AZ14</f>
         <v>0</v>
@@ -4729,34 +4729,34 @@
       <c r="N9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="186">
+      <c r="O9" s="185">
         <f>[1]REGISTRO!AF14</f>
         <v>0</v>
       </c>
-      <c r="P9" s="186"/>
+      <c r="P9" s="185"/>
     </row>
     <row r="10" spans="1:16" ht="20.399999999999999" customHeight="1">
-      <c r="A10" s="187" t="s">
+      <c r="A10" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="187"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="188">
+      <c r="B10" s="186"/>
+      <c r="C10" s="186"/>
+      <c r="D10" s="187">
         <f>[1]REGISTRO!H14</f>
         <v>0</v>
       </c>
-      <c r="E10" s="188"/>
-      <c r="F10" s="188"/>
-      <c r="G10" s="188"/>
-      <c r="H10" s="187" t="s">
+      <c r="E10" s="187"/>
+      <c r="F10" s="187"/>
+      <c r="G10" s="187"/>
+      <c r="H10" s="186" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="187"/>
-      <c r="J10" s="195">
+      <c r="I10" s="186"/>
+      <c r="J10" s="194">
         <f>[1]REGISTRO!I14</f>
         <v>0</v>
       </c>
-      <c r="K10" s="195"/>
+      <c r="K10" s="194"/>
       <c r="L10" s="17" t="s">
         <v>17</v>
       </c>
@@ -4767,68 +4767,68 @@
       <c r="N10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="163">
+      <c r="O10" s="162">
         <f>[1]REGISTRO!AJ14</f>
         <v>0</v>
       </c>
-      <c r="P10" s="163"/>
+      <c r="P10" s="162"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1">
-      <c r="A11" s="169" t="s">
+      <c r="A11" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="169"/>
-      <c r="C11" s="169"/>
-      <c r="D11" s="169"/>
-      <c r="E11" s="169"/>
-      <c r="F11" s="169"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="169"/>
-      <c r="I11" s="169"/>
-      <c r="J11" s="169"/>
-      <c r="K11" s="169"/>
-      <c r="L11" s="169"/>
-      <c r="M11" s="169"/>
-      <c r="N11" s="169"/>
-      <c r="O11" s="169"/>
-      <c r="P11" s="169"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="168"/>
+      <c r="G11" s="168"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="168"/>
+      <c r="J11" s="168"/>
+      <c r="K11" s="168"/>
+      <c r="L11" s="168"/>
+      <c r="M11" s="168"/>
+      <c r="N11" s="168"/>
+      <c r="O11" s="168"/>
+      <c r="P11" s="168"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1">
-      <c r="A12" s="170" t="s">
+      <c r="A12" s="169" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="172" t="s">
+      <c r="B12" s="171" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="174" t="s">
+      <c r="C12" s="173" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="176" t="s">
+      <c r="D12" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="177"/>
-      <c r="F12" s="176" t="s">
+      <c r="E12" s="176"/>
+      <c r="F12" s="175" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="178"/>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="177"/>
-      <c r="K12" s="176" t="s">
+      <c r="G12" s="177"/>
+      <c r="H12" s="177"/>
+      <c r="I12" s="177"/>
+      <c r="J12" s="176"/>
+      <c r="K12" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="178"/>
-      <c r="M12" s="178"/>
-      <c r="N12" s="177"/>
-      <c r="O12" s="179" t="s">
+      <c r="L12" s="177"/>
+      <c r="M12" s="177"/>
+      <c r="N12" s="176"/>
+      <c r="O12" s="178" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="180"/>
+      <c r="P12" s="179"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1">
-      <c r="A13" s="171"/>
-      <c r="B13" s="173"/>
-      <c r="C13" s="175"/>
+      <c r="A13" s="170"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="174"/>
       <c r="D13" s="19" t="s">
         <v>27</v>
       </c>
@@ -4862,8 +4862,8 @@
       <c r="N13" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="181"/>
-      <c r="P13" s="182"/>
+      <c r="O13" s="180"/>
+      <c r="P13" s="181"/>
     </row>
     <row r="14" spans="1:16" ht="14.4" customHeight="1">
       <c r="A14" s="23">
@@ -4922,11 +4922,11 @@
         <f>[1]REGISTRO!AR14</f>
         <v>0</v>
       </c>
-      <c r="O14" s="203">
+      <c r="O14" s="202">
         <f>[1]REGISTRO!BC14</f>
         <v>0</v>
       </c>
-      <c r="P14" s="204"/>
+      <c r="P14" s="203"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1">
       <c r="A15" s="34"/>
@@ -4967,8 +4967,8 @@
         <f>[1]REGISTRO!AS14</f>
         <v>0</v>
       </c>
-      <c r="O15" s="205"/>
-      <c r="P15" s="206"/>
+      <c r="O15" s="204"/>
+      <c r="P15" s="205"/>
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1">
       <c r="A16" s="48" t="s">
@@ -5005,19 +5005,19 @@
         <f>[1]REGISTRO!CJ14</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O16" s="205"/>
-      <c r="P16" s="206"/>
+      <c r="O16" s="204"/>
+      <c r="P16" s="205"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="55" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="209">
+      <c r="C17" s="208">
         <f>[1]REGISTRO!AT14</f>
         <v>0</v>
       </c>
-      <c r="D17" s="209"/>
+      <c r="D17" s="208"/>
       <c r="E17" s="5" t="s">
         <v>42</v>
       </c>
@@ -5042,8 +5042,8 @@
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="205"/>
-      <c r="P17" s="206"/>
+      <c r="O17" s="204"/>
+      <c r="P17" s="205"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1"/>
@@ -5060,19 +5060,19 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="205"/>
-      <c r="P18" s="206"/>
+      <c r="O18" s="204"/>
+      <c r="P18" s="205"/>
     </row>
     <row r="19" spans="1:16" ht="15" thickBot="1">
       <c r="A19" s="61" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="209">
+      <c r="C19" s="208">
         <f>[1]REGISTRO!AU14</f>
         <v>0</v>
       </c>
-      <c r="D19" s="209"/>
+      <c r="D19" s="208"/>
       <c r="E19" s="5" t="s">
         <v>42</v>
       </c>
@@ -5100,8 +5100,8 @@
         <v>0</v>
       </c>
       <c r="N19" s="1"/>
-      <c r="O19" s="207"/>
-      <c r="P19" s="208"/>
+      <c r="O19" s="206"/>
+      <c r="P19" s="207"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="61"/>
@@ -5127,24 +5127,24 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="57"/>
-      <c r="D21" s="210" t="s">
+      <c r="D21" s="209" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="210"/>
-      <c r="F21" s="210"/>
+      <c r="E21" s="209"/>
+      <c r="F21" s="209"/>
       <c r="G21" s="69"/>
-      <c r="H21" s="210" t="s">
+      <c r="H21" s="209" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="210"/>
-      <c r="J21" s="210"/>
+      <c r="I21" s="209"/>
+      <c r="J21" s="209"/>
       <c r="K21" s="70"/>
-      <c r="L21" s="210" t="s">
+      <c r="L21" s="209" t="s">
         <v>53</v>
       </c>
-      <c r="M21" s="210"/>
-      <c r="N21" s="210"/>
-      <c r="O21" s="210"/>
+      <c r="M21" s="209"/>
+      <c r="N21" s="209"/>
+      <c r="O21" s="209"/>
       <c r="P21" s="71"/>
     </row>
     <row r="22" spans="1:16" ht="18">
@@ -5246,13 +5246,13 @@
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="196">
+      <c r="M26" s="195">
         <f>[1]REGISTRO!K14</f>
         <v>0</v>
       </c>
-      <c r="N26" s="196"/>
-      <c r="O26" s="196"/>
-      <c r="P26" s="196"/>
+      <c r="N26" s="195"/>
+      <c r="O26" s="195"/>
+      <c r="P26" s="195"/>
     </row>
     <row r="27" spans="1:16" ht="14.4" customHeight="1">
       <c r="A27" s="1"/>
@@ -5267,10 +5267,10 @@
       <c r="J27" s="72"/>
       <c r="K27" s="10"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="196"/>
-      <c r="N27" s="196"/>
-      <c r="O27" s="196"/>
-      <c r="P27" s="196"/>
+      <c r="M27" s="195"/>
+      <c r="N27" s="195"/>
+      <c r="O27" s="195"/>
+      <c r="P27" s="195"/>
     </row>
     <row r="28" spans="1:16" ht="14.4" customHeight="1">
       <c r="A28" s="72"/>
@@ -5285,10 +5285,10 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="197"/>
-      <c r="N28" s="197"/>
-      <c r="O28" s="197"/>
-      <c r="P28" s="197"/>
+      <c r="M28" s="196"/>
+      <c r="N28" s="196"/>
+      <c r="O28" s="196"/>
+      <c r="P28" s="196"/>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="70"/>
@@ -5303,12 +5303,12 @@
       <c r="J29" s="78"/>
       <c r="K29" s="70"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="198" t="s">
+      <c r="M29" s="197" t="s">
         <v>61</v>
       </c>
-      <c r="N29" s="198"/>
-      <c r="O29" s="198"/>
-      <c r="P29" s="198"/>
+      <c r="N29" s="197"/>
+      <c r="O29" s="197"/>
+      <c r="P29" s="197"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="72" t="s">
@@ -5454,184 +5454,184 @@
     </row>
     <row r="37" spans="1:16" ht="14.4" customHeight="1">
       <c r="A37" s="89"/>
-      <c r="B37" s="199"/>
-      <c r="C37" s="199"/>
-      <c r="D37" s="200" t="s">
+      <c r="B37" s="198"/>
+      <c r="C37" s="198"/>
+      <c r="D37" s="199" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="200"/>
-      <c r="F37" s="200"/>
-      <c r="G37" s="200"/>
-      <c r="H37" s="200"/>
-      <c r="I37" s="200"/>
-      <c r="J37" s="200"/>
-      <c r="K37" s="201" t="s">
+      <c r="E37" s="199"/>
+      <c r="F37" s="199"/>
+      <c r="G37" s="199"/>
+      <c r="H37" s="199"/>
+      <c r="I37" s="199"/>
+      <c r="J37" s="199"/>
+      <c r="K37" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="L37" s="201"/>
-      <c r="M37" s="201"/>
-      <c r="N37" s="202">
+      <c r="L37" s="200"/>
+      <c r="M37" s="200"/>
+      <c r="N37" s="201">
         <f>+P4</f>
         <v>0</v>
       </c>
-      <c r="O37" s="202"/>
+      <c r="O37" s="201"/>
       <c r="P37" s="90"/>
     </row>
     <row r="38" spans="1:16" ht="14.4" customHeight="1">
       <c r="A38" s="89"/>
-      <c r="B38" s="199"/>
-      <c r="C38" s="199"/>
-      <c r="D38" s="200"/>
-      <c r="E38" s="200"/>
-      <c r="F38" s="200"/>
-      <c r="G38" s="200"/>
-      <c r="H38" s="200"/>
-      <c r="I38" s="200"/>
-      <c r="J38" s="200"/>
-      <c r="K38" s="201"/>
-      <c r="L38" s="201"/>
-      <c r="M38" s="201"/>
-      <c r="N38" s="202"/>
-      <c r="O38" s="202"/>
+      <c r="B38" s="198"/>
+      <c r="C38" s="198"/>
+      <c r="D38" s="199"/>
+      <c r="E38" s="199"/>
+      <c r="F38" s="199"/>
+      <c r="G38" s="199"/>
+      <c r="H38" s="199"/>
+      <c r="I38" s="199"/>
+      <c r="J38" s="199"/>
+      <c r="K38" s="200"/>
+      <c r="L38" s="200"/>
+      <c r="M38" s="200"/>
+      <c r="N38" s="201"/>
+      <c r="O38" s="201"/>
       <c r="P38" s="90"/>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A39" s="89"/>
-      <c r="B39" s="199"/>
-      <c r="C39" s="199"/>
-      <c r="D39" s="200"/>
-      <c r="E39" s="200"/>
-      <c r="F39" s="200"/>
-      <c r="G39" s="200"/>
-      <c r="H39" s="200"/>
-      <c r="I39" s="200"/>
-      <c r="J39" s="200"/>
-      <c r="K39" s="201"/>
-      <c r="L39" s="201"/>
-      <c r="M39" s="201"/>
-      <c r="N39" s="202"/>
-      <c r="O39" s="202"/>
+      <c r="B39" s="198"/>
+      <c r="C39" s="198"/>
+      <c r="D39" s="199"/>
+      <c r="E39" s="199"/>
+      <c r="F39" s="199"/>
+      <c r="G39" s="199"/>
+      <c r="H39" s="199"/>
+      <c r="I39" s="199"/>
+      <c r="J39" s="199"/>
+      <c r="K39" s="200"/>
+      <c r="L39" s="200"/>
+      <c r="M39" s="200"/>
+      <c r="N39" s="201"/>
+      <c r="O39" s="201"/>
       <c r="P39" s="90"/>
     </row>
     <row r="40" spans="1:16" ht="14.4" customHeight="1">
       <c r="A40" s="89"/>
-      <c r="B40" s="223" t="s">
+      <c r="B40" s="222" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="224"/>
-      <c r="D40" s="224" t="s">
+      <c r="C40" s="223"/>
+      <c r="D40" s="223" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="227" t="s">
+      <c r="E40" s="226" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="227"/>
-      <c r="G40" s="229" t="s">
+      <c r="F40" s="226"/>
+      <c r="G40" s="228" t="s">
         <v>73</v>
       </c>
-      <c r="H40" s="229"/>
-      <c r="I40" s="229" t="s">
+      <c r="H40" s="228"/>
+      <c r="I40" s="228" t="s">
         <v>74</v>
       </c>
-      <c r="J40" s="231"/>
-      <c r="K40" s="233" t="s">
+      <c r="J40" s="230"/>
+      <c r="K40" s="232" t="s">
         <v>75</v>
       </c>
-      <c r="L40" s="234"/>
-      <c r="M40" s="234"/>
-      <c r="N40" s="235"/>
-      <c r="O40" s="211" t="s">
+      <c r="L40" s="233"/>
+      <c r="M40" s="233"/>
+      <c r="N40" s="234"/>
+      <c r="O40" s="210" t="s">
         <v>76</v>
       </c>
       <c r="P40" s="90"/>
     </row>
     <row r="41" spans="1:16" ht="14.4" customHeight="1">
       <c r="A41" s="89"/>
-      <c r="B41" s="225"/>
-      <c r="C41" s="226"/>
-      <c r="D41" s="226"/>
-      <c r="E41" s="228"/>
-      <c r="F41" s="228"/>
-      <c r="G41" s="230"/>
-      <c r="H41" s="230"/>
-      <c r="I41" s="230"/>
-      <c r="J41" s="232"/>
-      <c r="K41" s="236"/>
-      <c r="L41" s="237"/>
-      <c r="M41" s="237"/>
-      <c r="N41" s="238"/>
-      <c r="O41" s="212"/>
+      <c r="B41" s="224"/>
+      <c r="C41" s="225"/>
+      <c r="D41" s="225"/>
+      <c r="E41" s="227"/>
+      <c r="F41" s="227"/>
+      <c r="G41" s="229"/>
+      <c r="H41" s="229"/>
+      <c r="I41" s="229"/>
+      <c r="J41" s="231"/>
+      <c r="K41" s="235"/>
+      <c r="L41" s="236"/>
+      <c r="M41" s="236"/>
+      <c r="N41" s="237"/>
+      <c r="O41" s="211"/>
       <c r="P41" s="90"/>
     </row>
     <row r="42" spans="1:16" ht="14.4" customHeight="1">
       <c r="A42" s="89"/>
-      <c r="B42" s="225"/>
-      <c r="C42" s="226"/>
-      <c r="D42" s="226"/>
-      <c r="E42" s="228"/>
-      <c r="F42" s="228"/>
-      <c r="G42" s="230"/>
-      <c r="H42" s="230"/>
-      <c r="I42" s="230"/>
-      <c r="J42" s="232"/>
-      <c r="K42" s="239"/>
-      <c r="L42" s="240"/>
-      <c r="M42" s="240"/>
-      <c r="N42" s="241"/>
-      <c r="O42" s="213"/>
+      <c r="B42" s="224"/>
+      <c r="C42" s="225"/>
+      <c r="D42" s="225"/>
+      <c r="E42" s="227"/>
+      <c r="F42" s="227"/>
+      <c r="G42" s="229"/>
+      <c r="H42" s="229"/>
+      <c r="I42" s="229"/>
+      <c r="J42" s="231"/>
+      <c r="K42" s="238"/>
+      <c r="L42" s="239"/>
+      <c r="M42" s="239"/>
+      <c r="N42" s="240"/>
+      <c r="O42" s="212"/>
       <c r="P42" s="90"/>
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="89"/>
-      <c r="B43" s="214"/>
-      <c r="C43" s="215"/>
-      <c r="D43" s="216"/>
-      <c r="E43" s="216"/>
-      <c r="F43" s="216"/>
-      <c r="G43" s="217"/>
-      <c r="H43" s="217"/>
-      <c r="I43" s="218"/>
-      <c r="J43" s="219"/>
-      <c r="K43" s="220"/>
-      <c r="L43" s="221"/>
-      <c r="M43" s="221"/>
-      <c r="N43" s="222"/>
+      <c r="B43" s="213"/>
+      <c r="C43" s="214"/>
+      <c r="D43" s="215"/>
+      <c r="E43" s="215"/>
+      <c r="F43" s="215"/>
+      <c r="G43" s="216"/>
+      <c r="H43" s="216"/>
+      <c r="I43" s="217"/>
+      <c r="J43" s="218"/>
+      <c r="K43" s="219"/>
+      <c r="L43" s="220"/>
+      <c r="M43" s="220"/>
+      <c r="N43" s="221"/>
       <c r="O43" s="94"/>
       <c r="P43" s="90"/>
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="89"/>
-      <c r="B44" s="214"/>
-      <c r="C44" s="215"/>
-      <c r="D44" s="216"/>
-      <c r="E44" s="216"/>
-      <c r="F44" s="216"/>
-      <c r="G44" s="217"/>
-      <c r="H44" s="217"/>
-      <c r="I44" s="218"/>
-      <c r="J44" s="219"/>
-      <c r="K44" s="220"/>
-      <c r="L44" s="221"/>
-      <c r="M44" s="221"/>
-      <c r="N44" s="222"/>
+      <c r="B44" s="213"/>
+      <c r="C44" s="214"/>
+      <c r="D44" s="215"/>
+      <c r="E44" s="215"/>
+      <c r="F44" s="215"/>
+      <c r="G44" s="216"/>
+      <c r="H44" s="216"/>
+      <c r="I44" s="217"/>
+      <c r="J44" s="218"/>
+      <c r="K44" s="219"/>
+      <c r="L44" s="220"/>
+      <c r="M44" s="220"/>
+      <c r="N44" s="221"/>
       <c r="O44" s="94"/>
       <c r="P44" s="90"/>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="89"/>
-      <c r="B45" s="214"/>
-      <c r="C45" s="215"/>
-      <c r="D45" s="216"/>
-      <c r="E45" s="216"/>
-      <c r="F45" s="216"/>
-      <c r="G45" s="217"/>
-      <c r="H45" s="217"/>
-      <c r="I45" s="218"/>
-      <c r="J45" s="219"/>
-      <c r="K45" s="220"/>
-      <c r="L45" s="221"/>
-      <c r="M45" s="221"/>
-      <c r="N45" s="222"/>
+      <c r="B45" s="213"/>
+      <c r="C45" s="214"/>
+      <c r="D45" s="215"/>
+      <c r="E45" s="215"/>
+      <c r="F45" s="215"/>
+      <c r="G45" s="216"/>
+      <c r="H45" s="216"/>
+      <c r="I45" s="217"/>
+      <c r="J45" s="218"/>
+      <c r="K45" s="219"/>
+      <c r="L45" s="220"/>
+      <c r="M45" s="220"/>
+      <c r="N45" s="221"/>
       <c r="O45" s="94"/>
       <c r="P45" s="90"/>
     </row>
@@ -5640,63 +5640,63 @@
       <c r="B46" s="95"/>
       <c r="C46" s="91"/>
       <c r="D46" s="91"/>
-      <c r="E46" s="199" t="s">
+      <c r="E46" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="F46" s="199"/>
-      <c r="G46" s="199" t="s">
+      <c r="F46" s="198"/>
+      <c r="G46" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="H46" s="199"/>
-      <c r="I46" s="199" t="s">
+      <c r="H46" s="198"/>
+      <c r="I46" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="J46" s="247"/>
-      <c r="K46" s="220"/>
-      <c r="L46" s="221"/>
-      <c r="M46" s="221"/>
-      <c r="N46" s="222"/>
+      <c r="J46" s="246"/>
+      <c r="K46" s="219"/>
+      <c r="L46" s="220"/>
+      <c r="M46" s="220"/>
+      <c r="N46" s="221"/>
       <c r="O46" s="94"/>
       <c r="P46" s="90"/>
     </row>
     <row r="47" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="89"/>
-      <c r="B47" s="248" t="s">
+      <c r="B47" s="247" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="249"/>
-      <c r="D47" s="249"/>
-      <c r="E47" s="249"/>
-      <c r="F47" s="249"/>
-      <c r="G47" s="249"/>
-      <c r="H47" s="249"/>
-      <c r="I47" s="249"/>
-      <c r="J47" s="250"/>
-      <c r="K47" s="253"/>
-      <c r="L47" s="254"/>
-      <c r="M47" s="254"/>
-      <c r="N47" s="255"/>
+      <c r="C47" s="248"/>
+      <c r="D47" s="248"/>
+      <c r="E47" s="248"/>
+      <c r="F47" s="248"/>
+      <c r="G47" s="248"/>
+      <c r="H47" s="248"/>
+      <c r="I47" s="248"/>
+      <c r="J47" s="249"/>
+      <c r="K47" s="252"/>
+      <c r="L47" s="253"/>
+      <c r="M47" s="253"/>
+      <c r="N47" s="254"/>
       <c r="O47" s="96"/>
       <c r="P47" s="90"/>
     </row>
     <row r="48" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A48" s="89"/>
-      <c r="B48" s="251"/>
-      <c r="C48" s="252"/>
-      <c r="D48" s="252"/>
-      <c r="E48" s="252"/>
-      <c r="F48" s="252"/>
-      <c r="G48" s="252"/>
-      <c r="H48" s="252"/>
-      <c r="I48" s="252"/>
-      <c r="J48" s="252"/>
-      <c r="K48" s="256" t="s">
+      <c r="B48" s="250"/>
+      <c r="C48" s="251"/>
+      <c r="D48" s="251"/>
+      <c r="E48" s="251"/>
+      <c r="F48" s="251"/>
+      <c r="G48" s="251"/>
+      <c r="H48" s="251"/>
+      <c r="I48" s="251"/>
+      <c r="J48" s="251"/>
+      <c r="K48" s="255" t="s">
         <v>79</v>
       </c>
-      <c r="L48" s="257"/>
-      <c r="M48" s="257"/>
-      <c r="N48" s="258"/>
-      <c r="O48" s="242" t="s">
+      <c r="L48" s="256"/>
+      <c r="M48" s="256"/>
+      <c r="N48" s="257"/>
+      <c r="O48" s="241" t="s">
         <v>80</v>
       </c>
       <c r="P48" s="90"/>
@@ -5712,11 +5712,11 @@
       <c r="H49" s="91"/>
       <c r="I49" s="89"/>
       <c r="J49" s="89"/>
-      <c r="K49" s="259"/>
-      <c r="L49" s="260"/>
-      <c r="M49" s="260"/>
-      <c r="N49" s="261"/>
-      <c r="O49" s="243"/>
+      <c r="K49" s="258"/>
+      <c r="L49" s="259"/>
+      <c r="M49" s="259"/>
+      <c r="N49" s="260"/>
+      <c r="O49" s="242"/>
       <c r="P49" s="90"/>
     </row>
     <row r="50" spans="1:16">
@@ -5730,10 +5730,10 @@
       <c r="H50" s="91"/>
       <c r="I50" s="89"/>
       <c r="J50" s="89"/>
-      <c r="K50" s="244"/>
-      <c r="L50" s="245"/>
-      <c r="M50" s="245"/>
-      <c r="N50" s="246"/>
+      <c r="K50" s="243"/>
+      <c r="L50" s="244"/>
+      <c r="M50" s="244"/>
+      <c r="N50" s="245"/>
       <c r="O50" s="97"/>
       <c r="P50" s="90"/>
     </row>
@@ -5748,10 +5748,10 @@
       <c r="H51" s="91"/>
       <c r="I51" s="89"/>
       <c r="J51" s="89"/>
-      <c r="K51" s="220"/>
-      <c r="L51" s="221"/>
-      <c r="M51" s="221"/>
-      <c r="N51" s="222"/>
+      <c r="K51" s="219"/>
+      <c r="L51" s="220"/>
+      <c r="M51" s="220"/>
+      <c r="N51" s="221"/>
       <c r="O51" s="94"/>
       <c r="P51" s="90"/>
     </row>
@@ -5765,30 +5765,30 @@
       <c r="G52" s="98"/>
       <c r="H52" s="91"/>
       <c r="I52" s="89"/>
-      <c r="J52" s="158" t="s">
+      <c r="J52" s="156" t="s">
         <v>106</v>
       </c>
-      <c r="K52" s="220"/>
-      <c r="L52" s="221"/>
-      <c r="M52" s="221"/>
-      <c r="N52" s="222"/>
+      <c r="K52" s="219"/>
+      <c r="L52" s="220"/>
+      <c r="M52" s="220"/>
+      <c r="N52" s="221"/>
       <c r="O52" s="94"/>
       <c r="P52" s="90"/>
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="89"/>
-      <c r="B53" s="156"/>
-      <c r="C53" s="156"/>
-      <c r="D53" s="156"/>
-      <c r="E53" s="156"/>
-      <c r="F53" s="156"/>
-      <c r="G53" s="156"/>
-      <c r="H53" s="156"/>
-      <c r="I53" s="157"/>
-      <c r="K53" s="220"/>
-      <c r="L53" s="221"/>
-      <c r="M53" s="221"/>
-      <c r="N53" s="222"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="89"/>
+      <c r="K53" s="219"/>
+      <c r="L53" s="220"/>
+      <c r="M53" s="220"/>
+      <c r="N53" s="221"/>
       <c r="O53" s="94"/>
       <c r="P53" s="90"/>
     </row>
@@ -5803,10 +5803,10 @@
       <c r="H54" s="91"/>
       <c r="I54" s="89"/>
       <c r="J54" s="89"/>
-      <c r="K54" s="220"/>
-      <c r="L54" s="221"/>
-      <c r="M54" s="221"/>
-      <c r="N54" s="222"/>
+      <c r="K54" s="219"/>
+      <c r="L54" s="220"/>
+      <c r="M54" s="220"/>
+      <c r="N54" s="221"/>
       <c r="O54" s="94"/>
       <c r="P54" s="90"/>
     </row>
@@ -5821,10 +5821,10 @@
       <c r="H55" s="91"/>
       <c r="I55" s="89"/>
       <c r="J55" s="89"/>
-      <c r="K55" s="220"/>
-      <c r="L55" s="221"/>
-      <c r="M55" s="221"/>
-      <c r="N55" s="222"/>
+      <c r="K55" s="219"/>
+      <c r="L55" s="220"/>
+      <c r="M55" s="220"/>
+      <c r="N55" s="221"/>
       <c r="O55" s="94"/>
       <c r="P55" s="90"/>
     </row>
@@ -5843,10 +5843,10 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="220"/>
-      <c r="L56" s="221"/>
-      <c r="M56" s="221"/>
-      <c r="N56" s="222"/>
+      <c r="K56" s="219"/>
+      <c r="L56" s="220"/>
+      <c r="M56" s="220"/>
+      <c r="N56" s="221"/>
       <c r="O56" s="94"/>
       <c r="P56" s="90"/>
     </row>
@@ -5865,10 +5865,10 @@
       <c r="J57" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="K57" s="253"/>
-      <c r="L57" s="254"/>
-      <c r="M57" s="254"/>
-      <c r="N57" s="255"/>
+      <c r="K57" s="252"/>
+      <c r="L57" s="253"/>
+      <c r="M57" s="253"/>
+      <c r="N57" s="254"/>
       <c r="O57" s="102"/>
       <c r="P57" s="90"/>
     </row>
@@ -5917,8 +5917,8 @@
       <c r="B60" s="91"/>
       <c r="C60" s="91"/>
       <c r="D60" s="91"/>
-      <c r="E60" s="199"/>
-      <c r="F60" s="199"/>
+      <c r="E60" s="198"/>
+      <c r="F60" s="198"/>
       <c r="G60" s="91"/>
       <c r="H60" s="91"/>
       <c r="I60" s="89"/>
@@ -5993,59 +5993,59 @@
       <c r="P63" s="1"/>
     </row>
     <row r="64" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A64" s="189" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="189"/>
-      <c r="C64" s="189"/>
-      <c r="D64" s="189"/>
-      <c r="E64" s="189"/>
-      <c r="F64" s="189"/>
-      <c r="G64" s="189"/>
-      <c r="H64" s="189"/>
-      <c r="I64" s="189"/>
-      <c r="J64" s="189"/>
-      <c r="K64" s="189"/>
-      <c r="L64" s="189"/>
-      <c r="M64" s="189"/>
-      <c r="N64" s="189"/>
+      <c r="A64" s="188" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="188"/>
+      <c r="C64" s="188"/>
+      <c r="D64" s="188"/>
+      <c r="E64" s="188"/>
+      <c r="F64" s="188"/>
+      <c r="G64" s="188"/>
+      <c r="H64" s="188"/>
+      <c r="I64" s="188"/>
+      <c r="J64" s="188"/>
+      <c r="K64" s="188"/>
+      <c r="L64" s="188"/>
+      <c r="M64" s="188"/>
+      <c r="N64" s="188"/>
       <c r="O64" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P64" s="267">
+      <c r="P64" s="266">
         <f>P4</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A65" s="162"/>
-      <c r="B65" s="162"/>
-      <c r="C65" s="162"/>
-      <c r="D65" s="269"/>
-      <c r="E65" s="269"/>
-      <c r="F65" s="164"/>
-      <c r="G65" s="164"/>
-      <c r="H65" s="164"/>
-      <c r="I65" s="164"/>
-      <c r="J65" s="270"/>
-      <c r="K65" s="270"/>
-      <c r="L65" s="270"/>
-      <c r="M65" s="270"/>
-      <c r="N65" s="270"/>
+      <c r="A65" s="161"/>
+      <c r="B65" s="161"/>
+      <c r="C65" s="161"/>
+      <c r="D65" s="268"/>
+      <c r="E65" s="268"/>
+      <c r="F65" s="163"/>
+      <c r="G65" s="163"/>
+      <c r="H65" s="163"/>
+      <c r="I65" s="163"/>
+      <c r="J65" s="269"/>
+      <c r="K65" s="269"/>
+      <c r="L65" s="269"/>
+      <c r="M65" s="269"/>
+      <c r="N65" s="269"/>
       <c r="O65" s="6"/>
-      <c r="P65" s="268"/>
+      <c r="P65" s="267"/>
     </row>
     <row r="66" spans="1:16" ht="25.2">
-      <c r="A66" s="162" t="s">
+      <c r="A66" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="162"/>
-      <c r="C66" s="162"/>
-      <c r="D66" s="262" t="e">
+      <c r="B66" s="161"/>
+      <c r="C66" s="161"/>
+      <c r="D66" s="261" t="e">
         <f>D7</f>
         <v>#REF!</v>
       </c>
-      <c r="E66" s="262"/>
+      <c r="E66" s="261"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
       <c r="H66" s="8" t="s">
@@ -6055,18 +6055,18 @@
         <f>I7</f>
         <v>0</v>
       </c>
-      <c r="J66" s="164" t="s">
+      <c r="J66" s="163" t="s">
         <v>7</v>
       </c>
-      <c r="K66" s="164"/>
-      <c r="L66" s="263">
+      <c r="K66" s="163"/>
+      <c r="L66" s="262">
         <f>L7</f>
         <v>0</v>
       </c>
-      <c r="M66" s="264"/>
-      <c r="N66" s="264"/>
-      <c r="O66" s="264"/>
-      <c r="P66" s="264"/>
+      <c r="M66" s="263"/>
+      <c r="N66" s="263"/>
+      <c r="O66" s="263"/>
+      <c r="P66" s="263"/>
     </row>
     <row r="67" spans="1:16" ht="20.399999999999999" customHeight="1">
       <c r="A67" s="10" t="s">
@@ -6074,30 +6074,30 @@
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="265">
+      <c r="D67" s="264">
         <f>D8</f>
         <v>0</v>
       </c>
-      <c r="E67" s="265"/>
+      <c r="E67" s="264"/>
       <c r="F67" s="108"/>
       <c r="G67" s="108"/>
       <c r="H67" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I67" s="167">
+      <c r="I67" s="166">
         <f>I8</f>
         <v>0</v>
       </c>
-      <c r="J67" s="167"/>
+      <c r="J67" s="166"/>
       <c r="K67" s="108"/>
-      <c r="L67" s="168">
+      <c r="L67" s="167">
         <f>L8</f>
         <v>0</v>
       </c>
-      <c r="M67" s="266"/>
-      <c r="N67" s="266"/>
-      <c r="O67" s="266"/>
-      <c r="P67" s="266"/>
+      <c r="M67" s="265"/>
+      <c r="N67" s="265"/>
+      <c r="O67" s="265"/>
+      <c r="P67" s="265"/>
     </row>
     <row r="68" spans="1:16" ht="30" customHeight="1">
       <c r="A68" s="10" t="s">
@@ -6108,26 +6108,26 @@
         <v>0</v>
       </c>
       <c r="C68" s="10"/>
-      <c r="D68" s="271" t="s">
+      <c r="D68" s="270" t="s">
         <v>89</v>
       </c>
-      <c r="E68" s="271"/>
+      <c r="E68" s="270"/>
       <c r="F68" s="110">
         <f>I9</f>
         <v>0</v>
       </c>
-      <c r="G68" s="185" t="s">
+      <c r="G68" s="184" t="s">
         <v>15</v>
       </c>
-      <c r="H68" s="272"/>
-      <c r="I68" s="272"/>
-      <c r="J68" s="188">
+      <c r="H68" s="271"/>
+      <c r="I68" s="271"/>
+      <c r="J68" s="187">
         <f>D10</f>
         <v>0</v>
       </c>
-      <c r="K68" s="188"/>
-      <c r="L68" s="188"/>
-      <c r="M68" s="188"/>
+      <c r="K68" s="187"/>
+      <c r="L68" s="187"/>
+      <c r="M68" s="187"/>
       <c r="N68" s="107"/>
       <c r="O68" s="105" t="s">
         <v>16</v>
@@ -6138,79 +6138,79 @@
       </c>
     </row>
     <row r="69" spans="1:16" ht="15" thickBot="1">
-      <c r="A69" s="273" t="s">
+      <c r="A69" s="272" t="s">
         <v>19</v>
       </c>
-      <c r="B69" s="273"/>
-      <c r="C69" s="273"/>
-      <c r="D69" s="273"/>
-      <c r="E69" s="273"/>
-      <c r="F69" s="273"/>
-      <c r="G69" s="273"/>
-      <c r="H69" s="273"/>
-      <c r="I69" s="273"/>
-      <c r="J69" s="273"/>
-      <c r="K69" s="273"/>
-      <c r="L69" s="273"/>
-      <c r="M69" s="273"/>
-      <c r="N69" s="273"/>
-      <c r="O69" s="273"/>
-      <c r="P69" s="273"/>
+      <c r="B69" s="272"/>
+      <c r="C69" s="272"/>
+      <c r="D69" s="272"/>
+      <c r="E69" s="272"/>
+      <c r="F69" s="272"/>
+      <c r="G69" s="272"/>
+      <c r="H69" s="272"/>
+      <c r="I69" s="272"/>
+      <c r="J69" s="272"/>
+      <c r="K69" s="272"/>
+      <c r="L69" s="272"/>
+      <c r="M69" s="272"/>
+      <c r="N69" s="272"/>
+      <c r="O69" s="272"/>
+      <c r="P69" s="272"/>
     </row>
     <row r="70" spans="1:16" ht="15" thickBot="1">
-      <c r="A70" s="274" t="s">
+      <c r="A70" s="273" t="s">
         <v>20</v>
       </c>
-      <c r="B70" s="276" t="s">
+      <c r="B70" s="275" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="277" t="s">
+      <c r="C70" s="276" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="278"/>
-      <c r="E70" s="279" t="s">
+      <c r="D70" s="277"/>
+      <c r="E70" s="278" t="s">
         <v>20</v>
       </c>
-      <c r="F70" s="281" t="s">
+      <c r="F70" s="280" t="s">
         <v>90</v>
       </c>
-      <c r="G70" s="281" t="s">
+      <c r="G70" s="280" t="s">
         <v>91</v>
       </c>
-      <c r="H70" s="287" t="s">
+      <c r="H70" s="282" t="s">
         <v>26</v>
       </c>
-      <c r="I70" s="288"/>
-      <c r="J70" s="288"/>
-      <c r="K70" s="288"/>
-      <c r="L70" s="288"/>
-      <c r="M70" s="288"/>
-      <c r="N70" s="288"/>
-      <c r="O70" s="288"/>
-      <c r="P70" s="289"/>
+      <c r="I70" s="283"/>
+      <c r="J70" s="283"/>
+      <c r="K70" s="283"/>
+      <c r="L70" s="283"/>
+      <c r="M70" s="283"/>
+      <c r="N70" s="283"/>
+      <c r="O70" s="283"/>
+      <c r="P70" s="284"/>
     </row>
     <row r="71" spans="1:16" ht="15" customHeight="1" thickBot="1">
-      <c r="A71" s="275"/>
-      <c r="B71" s="276"/>
-      <c r="C71" s="290" t="s">
+      <c r="A71" s="274"/>
+      <c r="B71" s="275"/>
+      <c r="C71" s="289" t="s">
         <v>27</v>
       </c>
-      <c r="D71" s="278"/>
-      <c r="E71" s="280"/>
-      <c r="F71" s="282"/>
-      <c r="G71" s="280"/>
-      <c r="H71" s="291">
+      <c r="D71" s="277"/>
+      <c r="E71" s="279"/>
+      <c r="F71" s="281"/>
+      <c r="G71" s="279"/>
+      <c r="H71" s="290">
         <f>O14</f>
         <v>0</v>
       </c>
-      <c r="I71" s="292"/>
-      <c r="J71" s="292"/>
-      <c r="K71" s="292"/>
-      <c r="L71" s="292"/>
-      <c r="M71" s="292"/>
-      <c r="N71" s="292"/>
-      <c r="O71" s="292"/>
-      <c r="P71" s="293"/>
+      <c r="I71" s="291"/>
+      <c r="J71" s="291"/>
+      <c r="K71" s="291"/>
+      <c r="L71" s="291"/>
+      <c r="M71" s="291"/>
+      <c r="N71" s="291"/>
+      <c r="O71" s="291"/>
+      <c r="P71" s="292"/>
     </row>
     <row r="72" spans="1:16" ht="20.399999999999999">
       <c r="A72" s="111">
@@ -6221,11 +6221,11 @@
         <f>B14</f>
         <v>0</v>
       </c>
-      <c r="C72" s="300">
+      <c r="C72" s="299">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="D72" s="301"/>
+      <c r="D72" s="300"/>
       <c r="E72" s="113">
         <f>E14</f>
         <v>0</v>
@@ -6238,15 +6238,15 @@
         <f>+H14</f>
         <v>0</v>
       </c>
-      <c r="H72" s="294"/>
-      <c r="I72" s="295"/>
-      <c r="J72" s="295"/>
-      <c r="K72" s="295"/>
-      <c r="L72" s="295"/>
-      <c r="M72" s="295"/>
-      <c r="N72" s="295"/>
-      <c r="O72" s="295"/>
-      <c r="P72" s="296"/>
+      <c r="H72" s="293"/>
+      <c r="I72" s="294"/>
+      <c r="J72" s="294"/>
+      <c r="K72" s="294"/>
+      <c r="L72" s="294"/>
+      <c r="M72" s="294"/>
+      <c r="N72" s="294"/>
+      <c r="O72" s="294"/>
+      <c r="P72" s="295"/>
     </row>
     <row r="73" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A73" s="116">
@@ -6257,11 +6257,11 @@
         <f>B15</f>
         <v>0</v>
       </c>
-      <c r="C73" s="302">
+      <c r="C73" s="301">
         <f>D15</f>
         <v>0</v>
       </c>
-      <c r="D73" s="303"/>
+      <c r="D73" s="302"/>
       <c r="E73" s="118">
         <f>E15</f>
         <v>0</v>
@@ -6274,15 +6274,15 @@
         <f>H15</f>
         <v>0</v>
       </c>
-      <c r="H73" s="297"/>
-      <c r="I73" s="298"/>
-      <c r="J73" s="298"/>
-      <c r="K73" s="298"/>
-      <c r="L73" s="298"/>
-      <c r="M73" s="298"/>
-      <c r="N73" s="298"/>
-      <c r="O73" s="298"/>
-      <c r="P73" s="299"/>
+      <c r="H73" s="296"/>
+      <c r="I73" s="297"/>
+      <c r="J73" s="297"/>
+      <c r="K73" s="297"/>
+      <c r="L73" s="297"/>
+      <c r="M73" s="297"/>
+      <c r="N73" s="297"/>
+      <c r="O73" s="297"/>
+      <c r="P73" s="298"/>
     </row>
     <row r="74" spans="1:16" ht="25.2">
       <c r="A74" s="10" t="s">
@@ -6309,11 +6309,11 @@
     <row r="75" spans="1:16" ht="25.2">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
-      <c r="C75" s="284">
+      <c r="C75" s="286">
         <f>F14</f>
         <v>0</v>
       </c>
-      <c r="D75" s="284"/>
+      <c r="D75" s="286"/>
       <c r="E75" s="121"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
@@ -6332,8 +6332,8 @@
         <v>94</v>
       </c>
       <c r="B76" s="10"/>
-      <c r="C76" s="284"/>
-      <c r="D76" s="284"/>
+      <c r="C76" s="286"/>
+      <c r="D76" s="286"/>
       <c r="E76" s="73"/>
       <c r="F76" s="10"/>
       <c r="G76" s="124"/>
@@ -6396,11 +6396,11 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
-      <c r="O78" s="283">
+      <c r="O78" s="285">
         <f>C19</f>
         <v>0</v>
       </c>
-      <c r="P78" s="283"/>
+      <c r="P78" s="285"/>
     </row>
     <row r="79" spans="1:16">
       <c r="A79" s="72" t="s">
@@ -6503,28 +6503,28 @@
       <c r="P83" s="1"/>
     </row>
     <row r="84" spans="1:16">
-      <c r="A84" s="189" t="s">
+      <c r="A84" s="188" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="189"/>
-      <c r="C84" s="189"/>
-      <c r="D84" s="189"/>
-      <c r="E84" s="189"/>
-      <c r="F84" s="189"/>
-      <c r="G84" s="189"/>
-      <c r="H84" s="189"/>
-      <c r="I84" s="189"/>
-      <c r="J84" s="189"/>
-      <c r="K84" s="189"/>
-      <c r="L84" s="189"/>
-      <c r="M84" s="189"/>
-      <c r="N84" s="189"/>
-      <c r="O84" s="189"/>
-      <c r="P84" s="189"/>
+      <c r="B84" s="188"/>
+      <c r="C84" s="188"/>
+      <c r="D84" s="188"/>
+      <c r="E84" s="188"/>
+      <c r="F84" s="188"/>
+      <c r="G84" s="188"/>
+      <c r="H84" s="188"/>
+      <c r="I84" s="188"/>
+      <c r="J84" s="188"/>
+      <c r="K84" s="188"/>
+      <c r="L84" s="188"/>
+      <c r="M84" s="188"/>
+      <c r="N84" s="188"/>
+      <c r="O84" s="188"/>
+      <c r="P84" s="188"/>
     </row>
     <row r="85" spans="1:16" ht="14.4" customHeight="1">
       <c r="A85" s="5"/>
-      <c r="B85" s="284">
+      <c r="B85" s="286">
         <f>B9</f>
         <v>0</v>
       </c>
@@ -6543,7 +6543,7 @@
       <c r="O85" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P85" s="285">
+      <c r="P85" s="287">
         <f>P4</f>
         <v>0</v>
       </c>
@@ -6552,33 +6552,33 @@
       <c r="A86" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B86" s="284"/>
+      <c r="B86" s="286"/>
       <c r="C86" s="10"/>
-      <c r="D86" s="269"/>
-      <c r="E86" s="269"/>
-      <c r="F86" s="164"/>
-      <c r="G86" s="164"/>
-      <c r="H86" s="164"/>
-      <c r="I86" s="164"/>
-      <c r="J86" s="270"/>
-      <c r="K86" s="270"/>
-      <c r="L86" s="270"/>
-      <c r="M86" s="270"/>
-      <c r="N86" s="270"/>
+      <c r="D86" s="268"/>
+      <c r="E86" s="268"/>
+      <c r="F86" s="163"/>
+      <c r="G86" s="163"/>
+      <c r="H86" s="163"/>
+      <c r="I86" s="163"/>
+      <c r="J86" s="269"/>
+      <c r="K86" s="269"/>
+      <c r="L86" s="269"/>
+      <c r="M86" s="269"/>
+      <c r="N86" s="269"/>
       <c r="O86" s="6"/>
-      <c r="P86" s="286"/>
+      <c r="P86" s="288"/>
     </row>
     <row r="87" spans="1:16" ht="32.4">
-      <c r="A87" s="304" t="s">
+      <c r="A87" s="303" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="304"/>
-      <c r="C87" s="304"/>
-      <c r="D87" s="305" t="e">
+      <c r="B87" s="303"/>
+      <c r="C87" s="303"/>
+      <c r="D87" s="304" t="e">
         <f>D7</f>
         <v>#REF!</v>
       </c>
-      <c r="E87" s="305"/>
+      <c r="E87" s="304"/>
       <c r="F87" s="130"/>
       <c r="G87" s="130"/>
       <c r="H87" s="130" t="s">
@@ -6588,18 +6588,18 @@
         <f>I7</f>
         <v>0</v>
       </c>
-      <c r="J87" s="306" t="s">
+      <c r="J87" s="305" t="s">
         <v>7</v>
       </c>
-      <c r="K87" s="306"/>
-      <c r="L87" s="307">
+      <c r="K87" s="305"/>
+      <c r="L87" s="306">
         <f>L7</f>
         <v>0</v>
       </c>
-      <c r="M87" s="307"/>
-      <c r="N87" s="307"/>
-      <c r="O87" s="307"/>
-      <c r="P87" s="307"/>
+      <c r="M87" s="306"/>
+      <c r="N87" s="306"/>
+      <c r="O87" s="306"/>
+      <c r="P87" s="306"/>
     </row>
     <row r="88" spans="1:16" ht="30.6" thickBot="1">
       <c r="A88" s="131"/>
@@ -6613,72 +6613,72 @@
       <c r="I88" s="131"/>
       <c r="J88" s="15"/>
       <c r="K88" s="132"/>
-      <c r="L88" s="266">
+      <c r="L88" s="265">
         <f>+L67</f>
         <v>0</v>
       </c>
-      <c r="M88" s="266"/>
-      <c r="N88" s="266"/>
-      <c r="O88" s="266"/>
-      <c r="P88" s="266"/>
+      <c r="M88" s="265"/>
+      <c r="N88" s="265"/>
+      <c r="O88" s="265"/>
+      <c r="P88" s="265"/>
     </row>
     <row r="89" spans="1:16" ht="16.2" thickBot="1">
       <c r="A89" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="B89" s="161" t="s">
+      <c r="B89" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="C89" s="161"/>
+      <c r="C89" s="160"/>
       <c r="D89" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="E89" s="161" t="s">
+      <c r="E89" s="160" t="s">
         <v>99</v>
       </c>
-      <c r="F89" s="161"/>
+      <c r="F89" s="160"/>
       <c r="G89" s="135" t="s">
         <v>29</v>
       </c>
       <c r="H89" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="I89" s="161" t="s">
+      <c r="I89" s="307" t="s">
         <v>100</v>
       </c>
-      <c r="J89" s="161"/>
-      <c r="K89" s="161" t="s">
+      <c r="J89" s="160"/>
+      <c r="K89" s="160" t="s">
         <v>101</v>
       </c>
-      <c r="L89" s="161"/>
-      <c r="M89" s="161" t="s">
+      <c r="L89" s="160"/>
+      <c r="M89" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="N89" s="161"/>
-      <c r="O89" s="161" t="s">
+      <c r="N89" s="160"/>
+      <c r="O89" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="P89" s="161"/>
+      <c r="P89" s="160"/>
     </row>
     <row r="90" spans="1:16" ht="35.4" thickBot="1">
       <c r="A90" s="136">
         <f>A14</f>
         <v>0</v>
       </c>
-      <c r="B90" s="311">
+      <c r="B90" s="310">
         <f>B14</f>
         <v>0</v>
       </c>
-      <c r="C90" s="311"/>
+      <c r="C90" s="310"/>
       <c r="D90" s="136">
         <f>C14</f>
         <v>0</v>
       </c>
-      <c r="E90" s="311">
+      <c r="E90" s="310">
         <f>J14</f>
         <v>0</v>
       </c>
-      <c r="F90" s="311"/>
+      <c r="F90" s="310"/>
       <c r="G90" s="137">
         <f>G14</f>
         <v>0</v>
@@ -6687,37 +6687,37 @@
         <f>H14</f>
         <v>0</v>
       </c>
-      <c r="I90" s="312">
+      <c r="I90" s="311">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="J90" s="313"/>
-      <c r="K90" s="311">
+      <c r="J90" s="312"/>
+      <c r="K90" s="310">
         <f>E14</f>
         <v>0</v>
       </c>
-      <c r="L90" s="311"/>
-      <c r="M90" s="311">
+      <c r="L90" s="310"/>
+      <c r="M90" s="310">
         <f>F14</f>
         <v>0</v>
       </c>
-      <c r="N90" s="311"/>
-      <c r="O90" s="311">
+      <c r="N90" s="310"/>
+      <c r="O90" s="310">
         <f>I14</f>
         <v>0</v>
       </c>
-      <c r="P90" s="311"/>
+      <c r="P90" s="310"/>
     </row>
     <row r="91" spans="1:16" ht="16.2" thickBot="1">
       <c r="A91" s="134">
         <f>A15</f>
         <v>0</v>
       </c>
-      <c r="B91" s="161">
+      <c r="B91" s="160">
         <f>B15</f>
         <v>0</v>
       </c>
-      <c r="C91" s="161"/>
+      <c r="C91" s="160"/>
       <c r="D91" s="134">
         <f>C15</f>
         <v>0</v>
@@ -6735,26 +6735,26 @@
         <f>H15</f>
         <v>0</v>
       </c>
-      <c r="I91" s="310">
+      <c r="I91" s="307">
         <f>D15</f>
         <v>0</v>
       </c>
-      <c r="J91" s="161"/>
-      <c r="K91" s="161">
+      <c r="J91" s="160"/>
+      <c r="K91" s="160">
         <f>E15</f>
         <v>0</v>
       </c>
-      <c r="L91" s="161"/>
+      <c r="L91" s="160"/>
       <c r="M91" s="308">
         <f>F15</f>
         <v>0</v>
       </c>
       <c r="N91" s="308"/>
-      <c r="O91" s="161">
+      <c r="O91" s="160">
         <f>I15</f>
         <v>0</v>
       </c>
-      <c r="P91" s="161"/>
+      <c r="P91" s="160"/>
     </row>
     <row r="92" spans="1:16" ht="15.6">
       <c r="A92" s="134"/>
@@ -6775,78 +6775,78 @@
       <c r="P92" s="134"/>
     </row>
     <row r="93" spans="1:16" ht="18" customHeight="1">
-      <c r="A93" s="161" t="s">
+      <c r="A93" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="161"/>
-      <c r="C93" s="161" t="s">
+      <c r="B93" s="160"/>
+      <c r="C93" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="D93" s="161"/>
-      <c r="E93" s="161" t="s">
+      <c r="D93" s="160"/>
+      <c r="E93" s="160" t="s">
         <v>35</v>
       </c>
-      <c r="F93" s="161"/>
-      <c r="G93" s="161" t="s">
+      <c r="F93" s="160"/>
+      <c r="G93" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="H93" s="161"/>
+      <c r="H93" s="160"/>
       <c r="I93" s="133"/>
       <c r="J93" s="133"/>
-      <c r="K93" s="318"/>
-      <c r="L93" s="318"/>
-      <c r="M93" s="311">
+      <c r="K93" s="317"/>
+      <c r="L93" s="317"/>
+      <c r="M93" s="310">
         <f>F16</f>
         <v>0</v>
       </c>
-      <c r="N93" s="311"/>
-      <c r="O93" s="311">
+      <c r="N93" s="310"/>
+      <c r="O93" s="310">
         <f>I16</f>
         <v>0</v>
       </c>
-      <c r="P93" s="311"/>
+      <c r="P93" s="310"/>
     </row>
     <row r="94" spans="1:16" ht="32.4" customHeight="1">
-      <c r="A94" s="160">
+      <c r="A94" s="159">
         <f>K14</f>
         <v>0</v>
       </c>
-      <c r="B94" s="160"/>
-      <c r="C94" s="160">
+      <c r="B94" s="159"/>
+      <c r="C94" s="159">
         <f>L14</f>
         <v>0</v>
       </c>
-      <c r="D94" s="160"/>
-      <c r="E94" s="160">
+      <c r="D94" s="159"/>
+      <c r="E94" s="159">
         <f>M14</f>
         <v>0</v>
       </c>
-      <c r="F94" s="160"/>
-      <c r="G94" s="160">
+      <c r="F94" s="159"/>
+      <c r="G94" s="159">
         <f>N14</f>
         <v>0</v>
       </c>
-      <c r="H94" s="160"/>
+      <c r="H94" s="159"/>
       <c r="I94" s="141"/>
       <c r="J94" s="141"/>
-      <c r="K94" s="318" t="s">
+      <c r="K94" s="317" t="s">
         <v>102</v>
       </c>
-      <c r="L94" s="318"/>
-      <c r="M94" s="311"/>
-      <c r="N94" s="311"/>
-      <c r="O94" s="311"/>
-      <c r="P94" s="311"/>
+      <c r="L94" s="317"/>
+      <c r="M94" s="310"/>
+      <c r="N94" s="310"/>
+      <c r="O94" s="310"/>
+      <c r="P94" s="310"/>
     </row>
     <row r="95" spans="1:16" ht="34.799999999999997">
-      <c r="A95" s="160"/>
-      <c r="B95" s="160"/>
-      <c r="C95" s="160"/>
-      <c r="D95" s="160"/>
-      <c r="E95" s="160"/>
-      <c r="F95" s="160"/>
-      <c r="G95" s="160"/>
-      <c r="H95" s="160"/>
+      <c r="A95" s="159"/>
+      <c r="B95" s="159"/>
+      <c r="C95" s="159"/>
+      <c r="D95" s="159"/>
+      <c r="E95" s="159"/>
+      <c r="F95" s="159"/>
+      <c r="G95" s="159"/>
+      <c r="H95" s="159"/>
       <c r="I95" s="141"/>
       <c r="J95" s="141"/>
       <c r="K95" s="133"/>
@@ -6857,26 +6857,26 @@
       <c r="P95" s="136"/>
     </row>
     <row r="96" spans="1:16" ht="34.799999999999997">
-      <c r="A96" s="315">
+      <c r="A96" s="314">
         <f>K15</f>
         <v>0</v>
       </c>
-      <c r="B96" s="315"/>
-      <c r="C96" s="315">
+      <c r="B96" s="314"/>
+      <c r="C96" s="314">
         <f>L15</f>
         <v>0</v>
       </c>
-      <c r="D96" s="315"/>
-      <c r="E96" s="315">
+      <c r="D96" s="314"/>
+      <c r="E96" s="314">
         <f>M15</f>
         <v>0</v>
       </c>
-      <c r="F96" s="315"/>
-      <c r="G96" s="316">
+      <c r="F96" s="314"/>
+      <c r="G96" s="315">
         <f>N15</f>
         <v>0</v>
       </c>
-      <c r="H96" s="315"/>
+      <c r="H96" s="314"/>
       <c r="I96" s="141"/>
       <c r="J96" s="141"/>
       <c r="K96" s="133"/>
@@ -6887,17 +6887,17 @@
       <c r="P96" s="136"/>
     </row>
     <row r="97" spans="1:16" ht="28.2" customHeight="1">
-      <c r="A97" s="317" t="s">
+      <c r="A97" s="316" t="s">
         <v>61</v>
       </c>
-      <c r="B97" s="317"/>
-      <c r="C97" s="317"/>
-      <c r="D97" s="316">
+      <c r="B97" s="316"/>
+      <c r="C97" s="316"/>
+      <c r="D97" s="315">
         <f>M26</f>
         <v>0</v>
       </c>
-      <c r="E97" s="316"/>
-      <c r="F97" s="316"/>
+      <c r="E97" s="315"/>
+      <c r="F97" s="315"/>
       <c r="G97" s="75"/>
       <c r="H97" s="142" t="s">
         <v>41</v>
@@ -6931,59 +6931,59 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="5"/>
-      <c r="H98" s="306" t="s">
+      <c r="H98" s="305" t="s">
         <v>46</v>
       </c>
-      <c r="I98" s="306"/>
-      <c r="J98" s="306"/>
-      <c r="K98" s="306"/>
-      <c r="L98" s="306"/>
-      <c r="M98" s="306"/>
-      <c r="N98" s="314">
+      <c r="I98" s="305"/>
+      <c r="J98" s="305"/>
+      <c r="K98" s="305"/>
+      <c r="L98" s="305"/>
+      <c r="M98" s="305"/>
+      <c r="N98" s="313">
         <f>C19</f>
         <v>0</v>
       </c>
-      <c r="O98" s="314"/>
-      <c r="P98" s="314"/>
+      <c r="O98" s="313"/>
+      <c r="P98" s="313"/>
     </row>
     <row r="99" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A99" s="159">
+      <c r="A99" s="158">
         <f>O14</f>
         <v>0</v>
       </c>
-      <c r="B99" s="159"/>
-      <c r="C99" s="159"/>
-      <c r="D99" s="159"/>
-      <c r="E99" s="159"/>
-      <c r="F99" s="159"/>
-      <c r="G99" s="159"/>
-      <c r="H99" s="159"/>
-      <c r="I99" s="159"/>
-      <c r="J99" s="159"/>
-      <c r="K99" s="159"/>
-      <c r="L99" s="159"/>
-      <c r="M99" s="159"/>
-      <c r="N99" s="159"/>
-      <c r="O99" s="159"/>
-      <c r="P99" s="159"/>
+      <c r="B99" s="158"/>
+      <c r="C99" s="158"/>
+      <c r="D99" s="158"/>
+      <c r="E99" s="158"/>
+      <c r="F99" s="158"/>
+      <c r="G99" s="158"/>
+      <c r="H99" s="158"/>
+      <c r="I99" s="158"/>
+      <c r="J99" s="158"/>
+      <c r="K99" s="158"/>
+      <c r="L99" s="158"/>
+      <c r="M99" s="158"/>
+      <c r="N99" s="158"/>
+      <c r="O99" s="158"/>
+      <c r="P99" s="158"/>
     </row>
     <row r="100" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A100" s="159"/>
-      <c r="B100" s="159"/>
-      <c r="C100" s="159"/>
-      <c r="D100" s="159"/>
-      <c r="E100" s="159"/>
-      <c r="F100" s="159"/>
-      <c r="G100" s="159"/>
-      <c r="H100" s="159"/>
-      <c r="I100" s="159"/>
-      <c r="J100" s="159"/>
-      <c r="K100" s="159"/>
-      <c r="L100" s="159"/>
-      <c r="M100" s="159"/>
-      <c r="N100" s="159"/>
-      <c r="O100" s="159"/>
-      <c r="P100" s="159"/>
+      <c r="A100" s="158"/>
+      <c r="B100" s="158"/>
+      <c r="C100" s="158"/>
+      <c r="D100" s="158"/>
+      <c r="E100" s="158"/>
+      <c r="F100" s="158"/>
+      <c r="G100" s="158"/>
+      <c r="H100" s="158"/>
+      <c r="I100" s="158"/>
+      <c r="J100" s="158"/>
+      <c r="K100" s="158"/>
+      <c r="L100" s="158"/>
+      <c r="M100" s="158"/>
+      <c r="N100" s="158"/>
+      <c r="O100" s="158"/>
+      <c r="P100" s="158"/>
     </row>
     <row r="101" spans="1:16" ht="20.399999999999999">
       <c r="A101" s="146"/>
@@ -7150,7 +7150,6 @@
     <mergeCell ref="D86:E86"/>
     <mergeCell ref="F86:I86"/>
     <mergeCell ref="J86:N86"/>
-    <mergeCell ref="H70:P70"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="H71:P73"/>
     <mergeCell ref="C72:D72"/>
@@ -7166,6 +7165,7 @@
     <mergeCell ref="E70:E71"/>
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:P70"/>
     <mergeCell ref="A66:C66"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="J66:K66"/>

</xml_diff>